<commit_message>
Converted Employer Integration Tests to XUnit
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application.IntegrationTests/Employer/Employer-MissingMandatory.xlsx
+++ b/src/Sfa.Tl.Matching.Application.IntegrationTests/Employer/Employer-MissingMandatory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\DFE\tl-matching\src\Sfa.Tl.Matching.Application.IntegrationTests\Employer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEC4271-4367-4182-B561-DD66DC7ADB31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F328669-965A-4236-AD5E-5964E70AF19E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Advanced Find View" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>9082609f-9cf8-e811-80e0-000d3a214f60</t>
-  </si>
-  <si>
     <t>Aware</t>
   </si>
   <si>
@@ -102,13 +99,16 @@
   </si>
   <si>
     <t>CompanyType</t>
+  </si>
+  <si>
+    <t>Employer-MissingMandatory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -495,15 +495,15 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.5546875" style="10" bestFit="1" customWidth="1"/>
@@ -514,7 +514,7 @@
     <col min="12" max="12" width="8.77734375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -552,25 +552,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3">
         <v>43439.620694444398</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="11" t="s">
+        <v>26</v>
+      </c>
       <c r="E2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>6</v>
@@ -579,16 +578,16 @@
         <v>7777744465</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="11"/>
       <c r="D3" s="11"/>
@@ -601,7 +600,7 @@
       <c r="K3" s="11"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="8">
+  <dataValidations count="8">
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="(Do Not Modify) Modified On must be in the correct date and time format." promptTitle="Date and time" prompt=" " sqref="C2:C1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
@@ -633,7 +632,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="List Value" error="AUPA must be selected from the drop-down list." promptTitle="Option set" prompt="Select a value from the drop-down list." xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>hiddenSheet!$A$2:$D$2</xm:f>
@@ -653,45 +652,45 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>